<commit_message>
Made them easier to read
Added 0x to them so they are read as hex
</commit_message>
<xml_diff>
--- a/Lab3/InstructionDict.xlsx
+++ b/Lab3/InstructionDict.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65AE2B17-3E5F-47DD-97B4-972CE90F9E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nykol\Desktop\CSE-140\Lab3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB43D558-8FE3-4B11-89A0-CBA44F572C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iType" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Operation</t>
   </si>
@@ -45,9 +50,6 @@
     <t>andi</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>beq</t>
   </si>
   <si>
@@ -66,30 +68,18 @@
     <t>lui</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>lw</t>
   </si>
   <si>
     <t>ori</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>slti</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>sltiu</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>sb</t>
   </si>
   <si>
@@ -102,9 +92,6 @@
     <t>sw</t>
   </si>
   <si>
-    <t>2b</t>
-  </si>
-  <si>
     <t>funct(hex)</t>
   </si>
   <si>
@@ -129,9 +116,6 @@
     <t>slt</t>
   </si>
   <si>
-    <t>2a</t>
-  </si>
-  <si>
     <t>sltu</t>
   </si>
   <si>
@@ -151,13 +135,88 @@
   </si>
   <si>
     <t>jal</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>0x8</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x25</t>
+  </si>
+  <si>
+    <t>0x2a</t>
+  </si>
+  <si>
+    <t>0x2b</t>
+  </si>
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>0x2</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0x9</t>
+  </si>
+  <si>
+    <t>0xc</t>
+  </si>
+  <si>
+    <t>0x4</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>0xf</t>
+  </si>
+  <si>
+    <t>0xd</t>
+  </si>
+  <si>
+    <t>0xa</t>
+  </si>
+  <si>
+    <t>0xb</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>0x3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,17 +593,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,140 +611,140 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -698,118 +757,118 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2">
-        <v>23</v>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -821,13 +880,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9165AFDE-DDBF-4847-ACD4-5D45BD36E792}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -835,39 +894,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>

</xml_diff>